<commit_message>
Control de Cambios Registrar Elmentos Acta
</commit_message>
<xml_diff>
--- a/blocks/inventarios/gestionActa/registrarElementoActa/archivo/archivo_elementos.xlsx
+++ b/blocks/inventarios/gestionActa/registrarElementoActa/archivo/archivo_elementos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="504" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos a Cargar" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="195">
   <si>
     <t>Nivel Inventarios</t>
   </si>
@@ -971,7 +971,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:P4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1043,119 +1043,49 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>41</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>250000</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="K2" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="N2" s="4" t="n">
-        <v>20</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="5"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>500000</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>2015</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="N3" s="4" t="n">
-        <v>15</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="5"/>
       <c r="P3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>500000</v>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>6</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1163,12 +1093,8 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1188,8 +1114,8 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="A2:P4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1407,7 +1333,7 @@
   <dimension ref="A1:G162"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="1" sqref="A2:P4 C41"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3733,7 +3659,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="1" sqref="A2:P4 A40"/>
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3818,7 +3744,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="A2:P4 B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3914,7 +3840,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="1" sqref="A2:P4 J22"/>
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>